<commit_message>
code is almost fixed
</commit_message>
<xml_diff>
--- a/output/LUAD_statistics_all.xlsx
+++ b/output/LUAD_statistics_all.xlsx
@@ -57,54 +57,54 @@
     <t>9</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>17</t>
   </si>
   <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>35</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
     <t>32</t>
   </si>
   <si>
@@ -219,36 +219,36 @@
     <t>Amplification CDK4</t>
   </si>
   <si>
+    <t>Mutation EGFR</t>
+  </si>
+  <si>
+    <t>Mutation KRAS</t>
+  </si>
+  <si>
     <t>Pattern OR_KRAS</t>
   </si>
   <si>
+    <t>Pattern OR_CDK4_TP53</t>
+  </si>
+  <si>
+    <t>Mutation SMARCA4</t>
+  </si>
+  <si>
+    <t>Mutation TP53</t>
+  </si>
+  <si>
+    <t>Mutation ATM</t>
+  </si>
+  <si>
     <t>Pattern OR_CDKN2A</t>
   </si>
   <si>
-    <t>Pattern OR_CDK4_TP53</t>
-  </si>
-  <si>
-    <t>Mutation EGFR</t>
-  </si>
-  <si>
-    <t>Mutation KRAS</t>
+    <t>Mutation NF1</t>
   </si>
   <si>
     <t>Pattern OR_EGFR_SMARCA4</t>
   </si>
   <si>
-    <t>Mutation TP53</t>
-  </si>
-  <si>
-    <t>Mutation ATM</t>
-  </si>
-  <si>
-    <t>Mutation NF1</t>
-  </si>
-  <si>
-    <t>Mutation SMARCA4</t>
-  </si>
-  <si>
     <t>Mutation KEAP1</t>
   </si>
   <si>
@@ -261,34 +261,34 @@
     <t>Amplification MDM2</t>
   </si>
   <si>
+    <t>Amplification EGFR</t>
+  </si>
+  <si>
+    <t>Amplification KRAS</t>
+  </si>
+  <si>
+    <t>Mutation STK11</t>
+  </si>
+  <si>
+    <t>Mutation NFE2L2</t>
+  </si>
+  <si>
+    <t>Mutation RB1</t>
+  </si>
+  <si>
     <t>Amplification CCND1</t>
   </si>
   <si>
-    <t>Amplification EGFR</t>
-  </si>
-  <si>
-    <t>Mutation STK11</t>
-  </si>
-  <si>
-    <t>Amplification KRAS</t>
+    <t>Mutation CDKN2A</t>
+  </si>
+  <si>
+    <t>Mutation RET</t>
   </si>
   <si>
     <t>Deletion CDKN2A</t>
   </si>
   <si>
-    <t>Mutation RB1</t>
-  </si>
-  <si>
     <t>Amplification MET</t>
-  </si>
-  <si>
-    <t>Mutation CDKN2A</t>
-  </si>
-  <si>
-    <t>Mutation NFE2L2</t>
-  </si>
-  <si>
-    <t>Mutation RET</t>
   </si>
   <si>
     <t>Mutation ROS1</t>
@@ -599,10 +599,10 @@
         <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0551797040169133</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N2" t="n">
-        <v>6.68557644855893E-4</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -613,13 +613,13 @@
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D3" t="n">
-        <v>158.0</v>
+        <v>65.0</v>
       </c>
       <c r="E3" t="n">
-        <v>46.0</v>
+        <v>28.0</v>
       </c>
       <c r="F3" t="n">
         <v>0.0058336561716597</v>
@@ -628,22 +628,22 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00131454955057744</v>
+        <v>3.24651120035433E-13</v>
       </c>
       <c r="I3" t="n">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
       <c r="J3" t="n">
         <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L3" t="n">
         <v>0.0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N3" t="n">
         <v>0.0</v>
@@ -657,13 +657,13 @@
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D4" t="n">
-        <v>103.0</v>
+        <v>141.0</v>
       </c>
       <c r="E4" t="n">
-        <v>19.0</v>
+        <v>34.0</v>
       </c>
       <c r="F4" t="n">
         <v>0.0059626167965088</v>
@@ -672,7 +672,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H4" t="n">
-        <v>8.46735787535546E-6</v>
+        <v>8.88220599278587E-4</v>
       </c>
       <c r="I4" t="n">
         <v>80.0</v>
@@ -681,13 +681,13 @@
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.040169133192389</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L4" t="n">
         <v>0.0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N4" t="n">
         <v>0.0</v>
@@ -701,13 +701,13 @@
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" t="n">
-        <v>265.0</v>
+        <v>158.0</v>
       </c>
       <c r="E5" t="n">
-        <v>28.0</v>
+        <v>84.0</v>
       </c>
       <c r="F5" t="n">
         <v>0.0059626167965088</v>
@@ -716,7 +716,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H5" t="n">
-        <v>1.77721953788421E-6</v>
+        <v>1.11208450607907E-5</v>
       </c>
       <c r="I5" t="n">
         <v>80.0</v>
@@ -725,13 +725,13 @@
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.17758985200845667</v>
       </c>
       <c r="L5" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N5" t="n">
         <v>0.0</v>
@@ -742,16 +742,16 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" t="n">
-        <v>158.0</v>
+        <v>265.0</v>
       </c>
       <c r="E6" t="n">
-        <v>84.0</v>
+        <v>28.0</v>
       </c>
       <c r="F6" t="n">
         <v>0.0059626167965088</v>
@@ -760,25 +760,25 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H6" t="n">
-        <v>1.11208450607907E-5</v>
+        <v>1.77721953788421E-6</v>
       </c>
       <c r="I6" t="n">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="J6" t="n">
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.17758985200845667</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L6" t="n">
         <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="7">
@@ -792,19 +792,19 @@
         <v>83</v>
       </c>
       <c r="D7" t="n">
-        <v>65.0</v>
+        <v>265.0</v>
       </c>
       <c r="E7" t="n">
-        <v>28.0</v>
+        <v>34.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G7" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H7" t="n">
-        <v>3.24651120035433E-13</v>
+        <v>8.27584277446678E-5</v>
       </c>
       <c r="I7" t="n">
         <v>60.0</v>
@@ -813,13 +813,13 @@
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L7" t="n">
         <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -830,25 +830,25 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D8" t="n">
-        <v>141.0</v>
+        <v>158.0</v>
       </c>
       <c r="E8" t="n">
-        <v>34.0</v>
+        <v>46.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G8" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H8" t="n">
-        <v>8.88220599278587E-4</v>
+        <v>0.00131454955057744</v>
       </c>
       <c r="I8" t="n">
         <v>60.0</v>
@@ -857,13 +857,13 @@
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N8" t="n">
         <v>0.0</v>
@@ -874,25 +874,25 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" t="n">
-        <v>120.0</v>
+        <v>48.0</v>
       </c>
       <c r="E9" t="n">
-        <v>82.0</v>
+        <v>15.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G9" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H9" t="n">
-        <v>4.12608987825272E-4</v>
+        <v>0.00161509241969472</v>
       </c>
       <c r="I9" t="n">
         <v>60.0</v>
@@ -901,13 +901,13 @@
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.173361522198731</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -918,10 +918,10 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" t="n">
         <v>250.0</v>
@@ -954,7 +954,7 @@
         <v>0.06553911205074</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0</v>
+        <v>6.5420519111824E-18</v>
       </c>
     </row>
     <row r="11">
@@ -962,10 +962,10 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D11" t="n">
         <v>46.0</v>
@@ -1006,25 +1006,25 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" t="n">
         <v>103.0</v>
       </c>
       <c r="E12" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G12" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00167276266869532</v>
+        <v>8.46735787535546E-6</v>
       </c>
       <c r="I12" t="n">
         <v>40.0</v>
@@ -1033,13 +1033,13 @@
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N12" t="n">
         <v>0.0</v>
@@ -1080,7 +1080,7 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M13" t="n">
         <v>0.0528541226215645</v>
@@ -1094,10 +1094,10 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" t="n">
         <v>250.0</v>
@@ -1130,7 +1130,7 @@
         <v>0.0528541226215645</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="15">
@@ -1138,25 +1138,25 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" t="n">
-        <v>48.0</v>
+        <v>265.0</v>
       </c>
       <c r="E15" t="n">
-        <v>15.0</v>
+        <v>23.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G15" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00161509241969472</v>
+        <v>9.13202144083936E-5</v>
       </c>
       <c r="I15" t="n">
         <v>40.0</v>
@@ -1165,13 +1165,13 @@
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L15" t="n">
         <v>0.0</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -1182,40 +1182,40 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D16" t="n">
-        <v>93.0</v>
+        <v>120.0</v>
       </c>
       <c r="E16" t="n">
-        <v>84.0</v>
+        <v>82.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.200982679178368</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G16" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H16" t="n">
-        <v>3.59155834889592E-4</v>
+        <v>4.12608987825272E-4</v>
       </c>
       <c r="I16" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="J16" t="n">
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.17758985200845667</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L16" t="n">
         <v>0.0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.177589852008457</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -1226,25 +1226,25 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" t="n">
-        <v>265.0</v>
+        <v>93.0</v>
       </c>
       <c r="E17" t="n">
-        <v>34.0</v>
+        <v>84.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.200982679178368</v>
       </c>
       <c r="G17" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H17" t="n">
-        <v>8.27584277446678E-5</v>
+        <v>3.59155834889592E-4</v>
       </c>
       <c r="I17" t="n">
         <v>20.0</v>
@@ -1253,13 +1253,13 @@
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.17758985200845667</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -1270,16 +1270,16 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
       </c>
       <c r="D18" t="n">
-        <v>265.0</v>
+        <v>103.0</v>
       </c>
       <c r="E18" t="n">
-        <v>23.0</v>
+        <v>15.0</v>
       </c>
       <c r="F18" t="n">
         <v>0.00396825396825397</v>
@@ -1288,7 +1288,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H18" t="n">
-        <v>9.13202144083936E-5</v>
+        <v>0.00167276266869532</v>
       </c>
       <c r="I18" t="n">
         <v>0.0</v>
@@ -1297,13 +1297,13 @@
         <v>100.0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L18" t="n">
         <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N18" t="n">
         <v>0.0</v>
@@ -1476,7 +1476,7 @@
         <v>0.12473572938689217</v>
       </c>
       <c r="L22" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M22" t="e">
         <v>#NUM!</v>
@@ -1564,7 +1564,7 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M24" t="e">
         <v>#NUM!</v>
@@ -1608,7 +1608,7 @@
         <v>0.06765327695560254</v>
       </c>
       <c r="L25" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>8.012344526598183E-18</v>
       </c>
       <c r="M25" t="e">
         <v>#NUM!</v>
@@ -1669,7 +1669,7 @@
         <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D27" t="e">
         <v>#NUM!</v>
@@ -1801,7 +1801,7 @@
         <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D30" t="e">
         <v>#NUM!</v>
@@ -1916,7 +1916,7 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>6.542051911182396E-18</v>
       </c>
       <c r="M32" t="e">
         <v>#NUM!</v>
@@ -2048,7 +2048,7 @@
         <v>0.07822410147991543</v>
       </c>
       <c r="L35" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M35" t="e">
         <v>#NUM!</v>
@@ -2109,7 +2109,7 @@
         <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D37" t="e">
         <v>#NUM!</v>
@@ -2153,7 +2153,7 @@
         <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" t="e">
         <v>#NUM!</v>
@@ -2285,7 +2285,7 @@
         <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D41" t="e">
         <v>#NUM!</v>
@@ -2329,7 +2329,7 @@
         <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D42" t="e">
         <v>#NUM!</v>
@@ -2441,10 +2441,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K44" t="n">
-        <v>0.493446088794926</v>
+        <v>0.4970401691331924</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0172102199975923</v>
+        <v>0.02016661652415717</v>
       </c>
       <c r="M44" t="e">
         <v>#NUM!</v>
@@ -2505,7 +2505,7 @@
         <v>80</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D46" t="e">
         <v>#NUM!</v>
@@ -2593,7 +2593,7 @@
         <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D48" t="e">
         <v>#NUM!</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>67</v>
@@ -3038,19 +3038,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D3" t="n">
-        <v>158.0</v>
+        <v>65.0</v>
       </c>
       <c r="E3" t="n">
-        <v>46.0</v>
+        <v>28.0</v>
       </c>
       <c r="F3" t="n">
         <v>0.0058336561716597</v>
@@ -3059,42 +3059,42 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00131454955057744</v>
+        <v>3.24651120035433E-13</v>
       </c>
       <c r="I3" t="n">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
       <c r="J3" t="n">
         <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L3" t="n">
         <v>0.0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.119450317124736</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0</v>
+        <v>0.00557131370713245</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D4" t="n">
-        <v>103.0</v>
+        <v>141.0</v>
       </c>
       <c r="E4" t="n">
-        <v>19.0</v>
+        <v>34.0</v>
       </c>
       <c r="F4" t="n">
         <v>0.0059626167965088</v>
@@ -3103,7 +3103,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H4" t="n">
-        <v>8.46735787535546E-6</v>
+        <v>8.88220599278587E-4</v>
       </c>
       <c r="I4" t="n">
         <v>80.0</v>
@@ -3112,13 +3112,13 @@
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.040169133192389</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L4" t="n">
         <v>0.0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N4" t="n">
         <v>0.0</v>
@@ -3126,19 +3126,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" t="n">
-        <v>265.0</v>
+        <v>158.0</v>
       </c>
       <c r="E5" t="n">
-        <v>28.0</v>
+        <v>84.0</v>
       </c>
       <c r="F5" t="n">
         <v>0.0059626167965088</v>
@@ -3147,7 +3147,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H5" t="n">
-        <v>1.77721953788421E-6</v>
+        <v>1.11208450607907E-5</v>
       </c>
       <c r="I5" t="n">
         <v>80.0</v>
@@ -3156,13 +3156,13 @@
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.17758985200845667</v>
       </c>
       <c r="L5" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N5" t="n">
         <v>0.0</v>
@@ -3170,19 +3170,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" t="n">
-        <v>158.0</v>
+        <v>265.0</v>
       </c>
       <c r="E6" t="n">
-        <v>84.0</v>
+        <v>28.0</v>
       </c>
       <c r="F6" t="n">
         <v>0.0059626167965088</v>
@@ -3191,22 +3191,22 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H6" t="n">
-        <v>1.11208450607907E-5</v>
+        <v>1.77721953788421E-6</v>
       </c>
       <c r="I6" t="n">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="J6" t="n">
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.17758985200845667</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L6" t="n">
         <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N6" t="n">
         <v>0.0</v>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>71</v>
@@ -3223,19 +3223,19 @@
         <v>83</v>
       </c>
       <c r="D7" t="n">
-        <v>65.0</v>
+        <v>265.0</v>
       </c>
       <c r="E7" t="n">
-        <v>28.0</v>
+        <v>34.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G7" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H7" t="n">
-        <v>3.24651120035433E-13</v>
+        <v>8.27584277446678E-5</v>
       </c>
       <c r="I7" t="n">
         <v>60.0</v>
@@ -3244,42 +3244,42 @@
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L7" t="n">
         <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.125581395348837</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N7" t="n">
-        <v>0.00469579457334959</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D8" t="n">
-        <v>141.0</v>
+        <v>158.0</v>
       </c>
       <c r="E8" t="n">
-        <v>34.0</v>
+        <v>46.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G8" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H8" t="n">
-        <v>8.88220599278587E-4</v>
+        <v>0.00131454955057744</v>
       </c>
       <c r="I8" t="n">
         <v>60.0</v>
@@ -3288,13 +3288,13 @@
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N8" t="n">
         <v>0.0</v>
@@ -3302,28 +3302,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" t="n">
-        <v>120.0</v>
+        <v>48.0</v>
       </c>
       <c r="E9" t="n">
-        <v>82.0</v>
+        <v>15.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G9" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H9" t="n">
-        <v>4.12608987825272E-4</v>
+        <v>0.00161509241969472</v>
       </c>
       <c r="I9" t="n">
         <v>60.0</v>
@@ -3332,13 +3332,13 @@
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.173361522198731</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -3349,10 +3349,10 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" t="n">
         <v>250.0</v>
@@ -3393,10 +3393,10 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D11" t="n">
         <v>46.0</v>
@@ -3434,28 +3434,28 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" t="n">
         <v>103.0</v>
       </c>
       <c r="E12" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G12" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00167276266869532</v>
+        <v>8.46735787535546E-6</v>
       </c>
       <c r="I12" t="n">
         <v>40.0</v>
@@ -3464,13 +3464,13 @@
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N12" t="n">
         <v>0.0</v>
@@ -3511,13 +3511,13 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M13" t="n">
         <v>0.0528541226215645</v>
       </c>
       <c r="N13" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -3525,10 +3525,10 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" t="n">
         <v>250.0</v>
@@ -3561,33 +3561,33 @@
         <v>0.0528541226215645</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" t="n">
-        <v>48.0</v>
+        <v>265.0</v>
       </c>
       <c r="E15" t="n">
-        <v>15.0</v>
+        <v>23.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G15" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00161509241969472</v>
+        <v>9.13202144083936E-5</v>
       </c>
       <c r="I15" t="n">
         <v>40.0</v>
@@ -3596,13 +3596,13 @@
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L15" t="n">
         <v>0.0</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -3610,43 +3610,43 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D16" t="n">
-        <v>93.0</v>
+        <v>120.0</v>
       </c>
       <c r="E16" t="n">
-        <v>84.0</v>
+        <v>82.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.200982679178368</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G16" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H16" t="n">
-        <v>3.59155834889592E-4</v>
+        <v>4.12608987825272E-4</v>
       </c>
       <c r="I16" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="J16" t="n">
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.17758985200845667</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L16" t="n">
         <v>0.0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.177589852008457</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -3654,28 +3654,28 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" t="n">
-        <v>265.0</v>
+        <v>93.0</v>
       </c>
       <c r="E17" t="n">
-        <v>34.0</v>
+        <v>84.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.200982679178368</v>
       </c>
       <c r="G17" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H17" t="n">
-        <v>8.27584277446678E-5</v>
+        <v>3.59155834889592E-4</v>
       </c>
       <c r="I17" t="n">
         <v>20.0</v>
@@ -3684,13 +3684,13 @@
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.17758985200845667</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -3698,13 +3698,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D18" t="n">
         <v>48.0</v>
@@ -3745,7 +3745,7 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
         <v>93</v>
@@ -3786,13 +3786,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" t="n">
         <v>266.0</v>
@@ -3825,18 +3825,18 @@
         <v>0.0591966173361522</v>
       </c>
       <c r="N20" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D21" t="n">
         <v>250.0</v>
@@ -3880,7 +3880,7 @@
         <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D22" t="n">
         <v>27.0</v>
@@ -3921,10 +3921,10 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D23" t="n">
         <v>250.0</v>
@@ -3962,43 +3962,43 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D24" t="n">
-        <v>93.0</v>
+        <v>103.0</v>
       </c>
       <c r="E24" t="n">
-        <v>59.0</v>
+        <v>15.0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0204179464513697</v>
+        <v>0.00167276266869532</v>
       </c>
       <c r="I24" t="n">
         <v>0.0</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K24" t="n">
-        <v>0.12473572938689217</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L24" t="n">
         <v>0.0</v>
       </c>
       <c r="M24" t="n">
-        <v>0.124735729386892</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N24" t="n">
         <v>0.0</v>
@@ -4006,16 +4006,16 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
         <v>94</v>
       </c>
       <c r="D25" t="n">
-        <v>158.0</v>
+        <v>93.0</v>
       </c>
       <c r="E25" t="n">
         <v>59.0</v>
@@ -4024,10 +4024,10 @@
         <v>0.0059626167965088</v>
       </c>
       <c r="G25" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00334798701112857</v>
+        <v>0.0204179464513697</v>
       </c>
       <c r="I25" t="n">
         <v>0.0</v>
@@ -4039,39 +4039,39 @@
         <v>0.12473572938689217</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M25" t="n">
         <v>0.124735729386892</v>
       </c>
       <c r="N25" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" t="n">
-        <v>64.0</v>
+        <v>158.0</v>
       </c>
       <c r="E26" t="n">
-        <v>37.0</v>
+        <v>59.0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G26" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H26" t="n">
-        <v>0.00333892782400472</v>
+        <v>0.00334798701112857</v>
       </c>
       <c r="I26" t="n">
         <v>0.0</v>
@@ -4080,30 +4080,30 @@
         <v>0.0</v>
       </c>
       <c r="K26" t="n">
-        <v>0.07822410147991543</v>
+        <v>0.12473572938689217</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0782241014799154</v>
+        <v>0.124735729386892</v>
       </c>
       <c r="N26" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
         <v>95</v>
       </c>
       <c r="D27" t="n">
-        <v>250.0</v>
+        <v>64.0</v>
       </c>
       <c r="E27" t="n">
         <v>37.0</v>
@@ -4112,10 +4112,10 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="G27" t="n">
-        <v>0.00793650793650794</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0641712118646901</v>
+        <v>0.00333892782400472</v>
       </c>
       <c r="I27" t="n">
         <v>0.0</v>
@@ -4138,28 +4138,28 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
         <v>95</v>
       </c>
-      <c r="C28" t="s">
-        <v>96</v>
-      </c>
       <c r="D28" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="E28" t="n">
         <v>37.0</v>
       </c>
-      <c r="E28" t="n">
-        <v>28.0</v>
-      </c>
       <c r="F28" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G28" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.00793650793650794</v>
       </c>
       <c r="H28" t="n">
-        <v>0.015920859802431</v>
+        <v>0.0641712118646901</v>
       </c>
       <c r="I28" t="n">
         <v>0.0</v>
@@ -4168,42 +4168,42 @@
         <v>0.0</v>
       </c>
       <c r="K28" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07822410147991543</v>
       </c>
       <c r="L28" t="n">
         <v>0.0</v>
       </c>
       <c r="M28" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0782241014799154</v>
       </c>
       <c r="N28" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
         <v>96</v>
       </c>
       <c r="D29" t="n">
-        <v>46.0</v>
+        <v>37.0</v>
       </c>
       <c r="E29" t="n">
         <v>28.0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="G29" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0142728080658903</v>
+        <v>0.015920859802431</v>
       </c>
       <c r="I29" t="n">
         <v>0.0</v>
@@ -4215,7 +4215,7 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L29" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M29" t="n">
         <v>0.0591966173361522</v>
@@ -4226,28 +4226,28 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
         <v>96</v>
       </c>
       <c r="D30" t="n">
-        <v>35.0</v>
+        <v>46.0</v>
       </c>
       <c r="E30" t="n">
         <v>28.0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0468463097466241</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G30" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0417860943528127</v>
+        <v>0.0142728080658903</v>
       </c>
       <c r="I30" t="n">
         <v>0.0</v>
@@ -4259,39 +4259,39 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L30" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M30" t="n">
         <v>0.0591966173361522</v>
       </c>
       <c r="N30" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
         <v>96</v>
       </c>
-      <c r="C31" t="s">
-        <v>79</v>
-      </c>
       <c r="D31" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="E31" t="n">
         <v>28.0</v>
       </c>
-      <c r="E31" t="n">
-        <v>25.0</v>
-      </c>
       <c r="F31" t="n">
-        <v>0.0277777777777778</v>
+        <v>0.0468463097466241</v>
       </c>
       <c r="G31" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H31" t="n">
-        <v>0.00528885616238524</v>
+        <v>0.0417860943528127</v>
       </c>
       <c r="I31" t="n">
         <v>0.0</v>
@@ -4300,13 +4300,13 @@
         <v>0.0</v>
       </c>
       <c r="K31" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L31" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M31" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N31" t="n">
         <v>0.0</v>
@@ -4314,28 +4314,28 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
         <v>79</v>
       </c>
       <c r="D32" t="n">
-        <v>31.0</v>
+        <v>28.0</v>
       </c>
       <c r="E32" t="n">
         <v>25.0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0277777777777778</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H32" t="n">
-        <v>0.00130554100709877</v>
+        <v>0.00528885616238524</v>
       </c>
       <c r="I32" t="n">
         <v>0.0</v>
@@ -4347,7 +4347,7 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M32" t="n">
         <v>0.0528541226215645</v>
@@ -4358,28 +4358,28 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D33" t="n">
-        <v>84.0</v>
+        <v>31.0</v>
       </c>
       <c r="E33" t="n">
-        <v>46.0</v>
+        <v>25.0</v>
       </c>
       <c r="F33" t="n">
         <v>0.0059626167965088</v>
       </c>
       <c r="G33" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H33" t="n">
-        <v>0.00153994324064719</v>
+        <v>0.00130554100709877</v>
       </c>
       <c r="I33" t="n">
         <v>0.0</v>
@@ -4388,13 +4388,13 @@
         <v>0.0</v>
       </c>
       <c r="K33" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L33" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N33" t="n">
         <v>0.0</v>
@@ -4402,28 +4402,28 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D34" t="n">
-        <v>31.0</v>
+        <v>84.0</v>
       </c>
       <c r="E34" t="n">
-        <v>25.0</v>
+        <v>46.0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0172268185197356</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H34" t="n">
-        <v>0.00352256830938948</v>
+        <v>0.00153994324064719</v>
       </c>
       <c r="I34" t="n">
         <v>0.0</v>
@@ -4432,13 +4432,13 @@
         <v>0.0</v>
       </c>
       <c r="K34" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L34" t="n">
         <v>0.0</v>
       </c>
       <c r="M34" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N34" t="n">
         <v>0.0</v>
@@ -4446,28 +4446,28 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D35" t="n">
-        <v>93.0</v>
+        <v>31.0</v>
       </c>
       <c r="E35" t="n">
-        <v>31.0</v>
+        <v>25.0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.0172268185197356</v>
       </c>
       <c r="G35" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0572545435376393</v>
+        <v>0.00352256830938948</v>
       </c>
       <c r="I35" t="n">
         <v>0.0</v>
@@ -4476,13 +4476,13 @@
         <v>0.0</v>
       </c>
       <c r="K35" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L35" t="n">
         <v>0.0</v>
       </c>
       <c r="M35" t="n">
-        <v>0.06553911205074</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N35" t="n">
         <v>0.0</v>
@@ -4490,28 +4490,28 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D36" t="n">
-        <v>250.0</v>
+        <v>93.0</v>
       </c>
       <c r="E36" t="n">
-        <v>64.0</v>
+        <v>31.0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G36" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0500405705476867</v>
+        <v>0.0572545435376393</v>
       </c>
       <c r="I36" t="n">
         <v>0.0</v>
@@ -4520,42 +4520,42 @@
         <v>0.0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.13530655391120508</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L36" t="n">
-        <v>0.0</v>
+        <v>6.542051911182396E-18</v>
       </c>
       <c r="M36" t="n">
-        <v>0.135306553911205</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="D37" t="n">
-        <v>37.0</v>
+        <v>250.0</v>
       </c>
       <c r="E37" t="n">
-        <v>27.0</v>
+        <v>64.0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.00798534817689006</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G37" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H37" t="n">
-        <v>0.00573068158794917</v>
+        <v>0.0500405705476867</v>
       </c>
       <c r="I37" t="n">
         <v>0.0</v>
@@ -4564,13 +4564,13 @@
         <v>0.0</v>
       </c>
       <c r="K37" t="n">
-        <v>0.05708245243128964</v>
+        <v>0.13530655391120508</v>
       </c>
       <c r="L37" t="n">
         <v>0.0</v>
       </c>
       <c r="M37" t="n">
-        <v>0.0570824524312896</v>
+        <v>0.135306553911205</v>
       </c>
       <c r="N37" t="n">
         <v>0.0</v>
@@ -4578,28 +4578,28 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
         <v>102</v>
       </c>
       <c r="D38" t="n">
-        <v>41.0</v>
+        <v>37.0</v>
       </c>
       <c r="E38" t="n">
         <v>27.0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.00793650793650794</v>
+        <v>0.00798534817689006</v>
       </c>
       <c r="G38" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H38" t="n">
-        <v>0.00496140462033587</v>
+        <v>0.00573068158794917</v>
       </c>
       <c r="I38" t="n">
         <v>0.0</v>
@@ -4617,33 +4617,33 @@
         <v>0.0570824524312896</v>
       </c>
       <c r="N38" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="D39" t="n">
-        <v>59.0</v>
+        <v>41.0</v>
       </c>
       <c r="E39" t="n">
-        <v>31.0</v>
+        <v>27.0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00793650793650794</v>
       </c>
       <c r="G39" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H39" t="n">
-        <v>0.00872783618701037</v>
+        <v>0.00496140462033587</v>
       </c>
       <c r="I39" t="n">
         <v>0.0</v>
@@ -4652,13 +4652,13 @@
         <v>0.0</v>
       </c>
       <c r="K39" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.05708245243128964</v>
       </c>
       <c r="L39" t="n">
         <v>0.0</v>
       </c>
       <c r="M39" t="n">
-        <v>0.06553911205074</v>
+        <v>0.0570824524312896</v>
       </c>
       <c r="N39" t="n">
         <v>0.0</v>
@@ -4666,16 +4666,16 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" t="n">
-        <v>78.0</v>
+        <v>59.0</v>
       </c>
       <c r="E40" t="n">
         <v>31.0</v>
@@ -4687,7 +4687,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0865916560787768</v>
+        <v>0.00872783618701037</v>
       </c>
       <c r="I40" t="n">
         <v>0.0</v>
@@ -4710,28 +4710,28 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D41" t="n">
-        <v>222.0</v>
+        <v>78.0</v>
       </c>
       <c r="E41" t="n">
-        <v>37.0</v>
+        <v>31.0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G41" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H41" t="n">
-        <v>0.00201437246540173</v>
+        <v>0.0865916560787768</v>
       </c>
       <c r="I41" t="n">
         <v>0.0</v>
@@ -4740,42 +4740,42 @@
         <v>0.0</v>
       </c>
       <c r="K41" t="n">
-        <v>0.07822410147991543</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L41" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M41" t="n">
-        <v>0.0782241014799154</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N41" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="D42" t="n">
-        <v>46.0</v>
+        <v>222.0</v>
       </c>
       <c r="E42" t="n">
-        <v>23.0</v>
+        <v>37.0</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G42" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H42" t="n">
-        <v>0.145038385111565</v>
+        <v>0.00201437246540173</v>
       </c>
       <c r="I42" t="n">
         <v>0.0</v>
@@ -4784,30 +4784,30 @@
         <v>0.0</v>
       </c>
       <c r="K42" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.07822410147991543</v>
       </c>
       <c r="L42" t="n">
         <v>0.0</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.0782241014799154</v>
       </c>
       <c r="N42" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D43" t="n">
-        <v>93.0</v>
+        <v>46.0</v>
       </c>
       <c r="E43" t="n">
         <v>23.0</v>
@@ -4816,10 +4816,10 @@
         <v>0.0059626167965088</v>
       </c>
       <c r="G43" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H43" t="n">
-        <v>0.0914870429913643</v>
+        <v>0.145038385111565</v>
       </c>
       <c r="I43" t="n">
         <v>0.0</v>
@@ -4842,34 +4842,34 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D44" t="n">
-        <v>265.0</v>
+        <v>93.0</v>
       </c>
       <c r="E44" t="n">
         <v>23.0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G44" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H44" t="n">
-        <v>9.13202144083936E-5</v>
+        <v>0.0914870429913643</v>
       </c>
       <c r="I44" t="n">
         <v>0.0</v>
       </c>
       <c r="J44" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K44" t="n">
         <v>0.048625792811839326</v>
@@ -4925,7 +4925,7 @@
         <v>0.0549682875264271</v>
       </c>
       <c r="N45" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
@@ -4969,7 +4969,7 @@
         <v>0.0549682875264271</v>
       </c>
       <c r="N46" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47">
@@ -4977,7 +4977,7 @@
         <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" t="s">
         <v>92</v>
@@ -5013,7 +5013,7 @@
         <v>0.0549682875264271</v>
       </c>
       <c r="N47" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="48">
@@ -5068,7 +5068,7 @@
         <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D49" t="n">
         <v>93.0</v>
@@ -5109,10 +5109,10 @@
         <v>133</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D50" t="n">
         <v>250.0</v>
@@ -5153,10 +5153,10 @@
         <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D51" t="n">
         <v>250.0</v>
@@ -5197,7 +5197,7 @@
         <v>135</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
         <v>107</v>
@@ -5241,10 +5241,10 @@
         <v>136</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D53" t="n">
         <v>250.0</v>
@@ -5285,7 +5285,7 @@
         <v>137</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C54" t="s">
         <v>117</v>
@@ -5326,7 +5326,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
         <v>80</v>
@@ -5370,7 +5370,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
         <v>80</v>
@@ -5403,7 +5403,7 @@
         <v>0.06765327695560254</v>
       </c>
       <c r="L56" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>8.012344526598183E-18</v>
       </c>
       <c r="M56" t="e">
         <v>#NUM!</v>
@@ -5464,7 +5464,7 @@
         <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D58" t="e">
         <v>#NUM!</v>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
         <v>80</v>
@@ -5590,13 +5590,13 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
         <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D61" t="e">
         <v>#NUM!</v>
@@ -5684,7 +5684,7 @@
         <v>80</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D63" t="e">
         <v>#NUM!</v>
@@ -5816,7 +5816,7 @@
         <v>80</v>
       </c>
       <c r="C66" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D66" t="e">
         <v>#NUM!</v>
@@ -5884,10 +5884,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K67" t="n">
-        <v>0.493446088794926</v>
+        <v>0.4970401691331924</v>
       </c>
       <c r="L67" t="n">
-        <v>0.0172102199975923</v>
+        <v>0.02016661652415717</v>
       </c>
       <c r="M67" t="e">
         <v>#NUM!</v>
@@ -5992,7 +5992,7 @@
         <v>80</v>
       </c>
       <c r="C70" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D70" t="e">
         <v>#NUM!</v>

</xml_diff>